<commit_message>
improve analysis of 103124 and 110724
</commit_message>
<xml_diff>
--- a/PFF_HTRA1/103124_analysis_by_cell.xlsx
+++ b/PFF_HTRA1/103124_analysis_by_cell.xlsx
@@ -933,16 +933,16 @@
         <v>2192</v>
       </c>
       <c r="D20" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E20" t="n">
-        <v>590</v>
+        <v>0</v>
       </c>
       <c r="F20" t="n">
         <v>3</v>
       </c>
       <c r="G20" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21">
@@ -1383,16 +1383,16 @@
         <v>14749</v>
       </c>
       <c r="D38" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E38" t="n">
-        <v>2356</v>
+        <v>0</v>
       </c>
       <c r="F38" t="n">
         <v>875</v>
       </c>
       <c r="G38" t="n">
-        <v>141</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39">
@@ -1408,16 +1408,16 @@
         <v>5031</v>
       </c>
       <c r="D39" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E39" t="n">
-        <v>782</v>
+        <v>0</v>
       </c>
       <c r="F39" t="n">
         <v>2233</v>
       </c>
       <c r="G39" t="n">
-        <v>449</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40">
@@ -1814,10 +1814,10 @@
         <v>254</v>
       </c>
       <c r="F55" t="n">
-        <v>3137</v>
+        <v>0</v>
       </c>
       <c r="G55" t="n">
-        <v>55</v>
+        <v>0</v>
       </c>
     </row>
     <row r="56">
@@ -1839,7 +1839,7 @@
         <v>0</v>
       </c>
       <c r="F56" t="n">
-        <v>4227</v>
+        <v>0</v>
       </c>
       <c r="G56" t="n">
         <v>0</v>
@@ -1864,10 +1864,10 @@
         <v>259</v>
       </c>
       <c r="F57" t="n">
-        <v>4075</v>
+        <v>0</v>
       </c>
       <c r="G57" t="n">
-        <v>201</v>
+        <v>0</v>
       </c>
     </row>
     <row r="58">
@@ -1889,7 +1889,7 @@
         <v>0</v>
       </c>
       <c r="F58" t="n">
-        <v>3945</v>
+        <v>0</v>
       </c>
       <c r="G58" t="n">
         <v>0</v>
@@ -1914,10 +1914,10 @@
         <v>283</v>
       </c>
       <c r="F59" t="n">
-        <v>4042</v>
+        <v>0</v>
       </c>
       <c r="G59" t="n">
-        <v>157</v>
+        <v>0</v>
       </c>
     </row>
     <row r="60">
@@ -1939,10 +1939,10 @@
         <v>1392</v>
       </c>
       <c r="F60" t="n">
-        <v>194</v>
+        <v>0</v>
       </c>
       <c r="G60" t="n">
-        <v>26</v>
+        <v>0</v>
       </c>
     </row>
     <row r="61">
@@ -1964,7 +1964,7 @@
         <v>0</v>
       </c>
       <c r="F61" t="n">
-        <v>97</v>
+        <v>0</v>
       </c>
       <c r="G61" t="n">
         <v>0</v>
@@ -2014,7 +2014,7 @@
         <v>0</v>
       </c>
       <c r="F63" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G63" t="n">
         <v>0</v>
@@ -2039,7 +2039,7 @@
         <v>269</v>
       </c>
       <c r="F64" t="n">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="G64" t="n">
         <v>0</v>
@@ -2064,7 +2064,7 @@
         <v>0</v>
       </c>
       <c r="F65" t="n">
-        <v>161</v>
+        <v>0</v>
       </c>
       <c r="G65" t="n">
         <v>0</v>
@@ -2114,7 +2114,7 @@
         <v>0</v>
       </c>
       <c r="F67" t="n">
-        <v>192</v>
+        <v>0</v>
       </c>
       <c r="G67" t="n">
         <v>0</v>
@@ -2139,7 +2139,7 @@
         <v>0</v>
       </c>
       <c r="F68" t="n">
-        <v>225</v>
+        <v>0</v>
       </c>
       <c r="G68" t="n">
         <v>0</v>
@@ -2164,10 +2164,10 @@
         <v>353</v>
       </c>
       <c r="F69" t="n">
-        <v>38</v>
+        <v>0</v>
       </c>
       <c r="G69" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="70">
@@ -2214,10 +2214,10 @@
         <v>133</v>
       </c>
       <c r="F71" t="n">
-        <v>2404</v>
+        <v>0</v>
       </c>
       <c r="G71" t="n">
-        <v>94</v>
+        <v>0</v>
       </c>
     </row>
     <row r="72">
@@ -2239,10 +2239,10 @@
         <v>209</v>
       </c>
       <c r="F72" t="n">
-        <v>3827</v>
+        <v>0</v>
       </c>
       <c r="G72" t="n">
-        <v>62</v>
+        <v>0</v>
       </c>
     </row>
     <row r="73">
@@ -2264,10 +2264,10 @@
         <v>3144</v>
       </c>
       <c r="F73" t="n">
-        <v>5458</v>
+        <v>0</v>
       </c>
       <c r="G73" t="n">
-        <v>989</v>
+        <v>0</v>
       </c>
     </row>
     <row r="74">
@@ -2289,7 +2289,7 @@
         <v>0</v>
       </c>
       <c r="F74" t="n">
-        <v>2719</v>
+        <v>0</v>
       </c>
       <c r="G74" t="n">
         <v>0</v>
@@ -2314,7 +2314,7 @@
         <v>0</v>
       </c>
       <c r="F75" t="n">
-        <v>3494</v>
+        <v>0</v>
       </c>
       <c r="G75" t="n">
         <v>0</v>
@@ -2339,10 +2339,10 @@
         <v>361</v>
       </c>
       <c r="F76" t="n">
-        <v>7481</v>
+        <v>0</v>
       </c>
       <c r="G76" t="n">
-        <v>313</v>
+        <v>0</v>
       </c>
     </row>
     <row r="77">
@@ -2364,7 +2364,7 @@
         <v>0</v>
       </c>
       <c r="F77" t="n">
-        <v>2431</v>
+        <v>0</v>
       </c>
       <c r="G77" t="n">
         <v>0</v>
@@ -2389,7 +2389,7 @@
         <v>0</v>
       </c>
       <c r="F78" t="n">
-        <v>3153</v>
+        <v>0</v>
       </c>
       <c r="G78" t="n">
         <v>0</v>
@@ -2414,7 +2414,7 @@
         <v>0</v>
       </c>
       <c r="F79" t="n">
-        <v>3247</v>
+        <v>0</v>
       </c>
       <c r="G79" t="n">
         <v>0</v>
@@ -2439,7 +2439,7 @@
         <v>0</v>
       </c>
       <c r="F80" t="n">
-        <v>5813</v>
+        <v>0</v>
       </c>
       <c r="G80" t="n">
         <v>0</v>
@@ -2464,10 +2464,10 @@
         <v>513</v>
       </c>
       <c r="F81" t="n">
-        <v>13480</v>
+        <v>0</v>
       </c>
       <c r="G81" t="n">
-        <v>247</v>
+        <v>0</v>
       </c>
     </row>
     <row r="82">
@@ -2489,10 +2489,10 @@
         <v>162</v>
       </c>
       <c r="F82" t="n">
-        <v>8369</v>
+        <v>0</v>
       </c>
       <c r="G82" t="n">
-        <v>75</v>
+        <v>0</v>
       </c>
     </row>
     <row r="83">
@@ -2514,7 +2514,7 @@
         <v>0</v>
       </c>
       <c r="F83" t="n">
-        <v>4943</v>
+        <v>0</v>
       </c>
       <c r="G83" t="n">
         <v>0</v>
@@ -2539,7 +2539,7 @@
         <v>0</v>
       </c>
       <c r="F84" t="n">
-        <v>6781</v>
+        <v>0</v>
       </c>
       <c r="G84" t="n">
         <v>0</v>
@@ -2564,7 +2564,7 @@
         <v>0</v>
       </c>
       <c r="F85" t="n">
-        <v>1413</v>
+        <v>0</v>
       </c>
       <c r="G85" t="n">
         <v>0</v>
@@ -2589,10 +2589,10 @@
         <v>2451</v>
       </c>
       <c r="F86" t="n">
-        <v>374</v>
+        <v>0</v>
       </c>
       <c r="G86" t="n">
-        <v>104</v>
+        <v>0</v>
       </c>
     </row>
     <row r="87">
@@ -2614,7 +2614,7 @@
         <v>0</v>
       </c>
       <c r="F87" t="n">
-        <v>52</v>
+        <v>0</v>
       </c>
       <c r="G87" t="n">
         <v>0</v>
@@ -2689,7 +2689,7 @@
         <v>0</v>
       </c>
       <c r="F90" t="n">
-        <v>332</v>
+        <v>0</v>
       </c>
       <c r="G90" t="n">
         <v>0</v>
@@ -2714,7 +2714,7 @@
         <v>0</v>
       </c>
       <c r="F91" t="n">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="G91" t="n">
         <v>0</v>
@@ -2739,7 +2739,7 @@
         <v>0</v>
       </c>
       <c r="F92" t="n">
-        <v>548</v>
+        <v>0</v>
       </c>
       <c r="G92" t="n">
         <v>0</v>
@@ -2764,7 +2764,7 @@
         <v>0</v>
       </c>
       <c r="F93" t="n">
-        <v>64</v>
+        <v>0</v>
       </c>
       <c r="G93" t="n">
         <v>0</v>
@@ -2789,10 +2789,10 @@
         <v>1906</v>
       </c>
       <c r="F94" t="n">
-        <v>3584</v>
+        <v>0</v>
       </c>
       <c r="G94" t="n">
-        <v>581</v>
+        <v>0</v>
       </c>
     </row>
     <row r="95">
@@ -2814,10 +2814,10 @@
         <v>32</v>
       </c>
       <c r="F95" t="n">
-        <v>3680</v>
+        <v>0</v>
       </c>
       <c r="G95" t="n">
-        <v>19</v>
+        <v>0</v>
       </c>
     </row>
     <row r="96">
@@ -2839,7 +2839,7 @@
         <v>0</v>
       </c>
       <c r="F96" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="G96" t="n">
         <v>0</v>
@@ -2864,10 +2864,10 @@
         <v>2337</v>
       </c>
       <c r="F97" t="n">
-        <v>32</v>
+        <v>0</v>
       </c>
       <c r="G97" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="98">
@@ -3258,16 +3258,16 @@
         <v>3237</v>
       </c>
       <c r="D113" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E113" t="n">
-        <v>714</v>
+        <v>0</v>
       </c>
       <c r="F113" t="n">
         <v>382</v>
       </c>
       <c r="G113" t="n">
-        <v>36</v>
+        <v>0</v>
       </c>
     </row>
     <row r="114">
@@ -4164,10 +4164,10 @@
         <v>6011</v>
       </c>
       <c r="F149" t="n">
-        <v>14634</v>
+        <v>0</v>
       </c>
       <c r="G149" t="n">
-        <v>2745</v>
+        <v>0</v>
       </c>
     </row>
     <row r="150">
@@ -4189,10 +4189,10 @@
         <v>73</v>
       </c>
       <c r="F150" t="n">
-        <v>14610</v>
+        <v>0</v>
       </c>
       <c r="G150" t="n">
-        <v>48</v>
+        <v>0</v>
       </c>
     </row>
     <row r="151">
@@ -4214,10 +4214,10 @@
         <v>277</v>
       </c>
       <c r="F151" t="n">
-        <v>7967</v>
+        <v>0</v>
       </c>
       <c r="G151" t="n">
-        <v>107</v>
+        <v>0</v>
       </c>
     </row>
     <row r="152">
@@ -4239,7 +4239,7 @@
         <v>0</v>
       </c>
       <c r="F152" t="n">
-        <v>8392</v>
+        <v>0</v>
       </c>
       <c r="G152" t="n">
         <v>0</v>
@@ -4264,7 +4264,7 @@
         <v>0</v>
       </c>
       <c r="F153" t="n">
-        <v>4494</v>
+        <v>0</v>
       </c>
       <c r="G153" t="n">
         <v>0</v>
@@ -4289,7 +4289,7 @@
         <v>0</v>
       </c>
       <c r="F154" t="n">
-        <v>4939</v>
+        <v>0</v>
       </c>
       <c r="G154" t="n">
         <v>0</v>
@@ -4314,10 +4314,10 @@
         <v>553</v>
       </c>
       <c r="F155" t="n">
-        <v>6312</v>
+        <v>0</v>
       </c>
       <c r="G155" t="n">
-        <v>554</v>
+        <v>0</v>
       </c>
     </row>
     <row r="156">
@@ -4339,10 +4339,10 @@
         <v>1373</v>
       </c>
       <c r="F156" t="n">
-        <v>5056</v>
+        <v>0</v>
       </c>
       <c r="G156" t="n">
-        <v>602</v>
+        <v>0</v>
       </c>
     </row>
     <row r="157">
@@ -4364,10 +4364,10 @@
         <v>908</v>
       </c>
       <c r="F157" t="n">
-        <v>6465</v>
+        <v>0</v>
       </c>
       <c r="G157" t="n">
-        <v>639</v>
+        <v>0</v>
       </c>
     </row>
     <row r="158">
@@ -4389,7 +4389,7 @@
         <v>0</v>
       </c>
       <c r="F158" t="n">
-        <v>5334</v>
+        <v>0</v>
       </c>
       <c r="G158" t="n">
         <v>0</v>
@@ -4414,7 +4414,7 @@
         <v>0</v>
       </c>
       <c r="F159" t="n">
-        <v>4805</v>
+        <v>0</v>
       </c>
       <c r="G159" t="n">
         <v>0</v>
@@ -4439,10 +4439,10 @@
         <v>421</v>
       </c>
       <c r="F160" t="n">
-        <v>6877</v>
+        <v>0</v>
       </c>
       <c r="G160" t="n">
-        <v>260</v>
+        <v>0</v>
       </c>
     </row>
     <row r="161">
@@ -4464,10 +4464,10 @@
         <v>2594</v>
       </c>
       <c r="F161" t="n">
-        <v>5336</v>
+        <v>0</v>
       </c>
       <c r="G161" t="n">
-        <v>1365</v>
+        <v>0</v>
       </c>
     </row>
     <row r="162">
@@ -4489,10 +4489,10 @@
         <v>399</v>
       </c>
       <c r="F162" t="n">
-        <v>6637</v>
+        <v>0</v>
       </c>
       <c r="G162" t="n">
-        <v>287</v>
+        <v>0</v>
       </c>
     </row>
     <row r="163">
@@ -4514,7 +4514,7 @@
         <v>0</v>
       </c>
       <c r="F163" t="n">
-        <v>4313</v>
+        <v>0</v>
       </c>
       <c r="G163" t="n">
         <v>0</v>
@@ -4539,7 +4539,7 @@
         <v>0</v>
       </c>
       <c r="F164" t="n">
-        <v>2657</v>
+        <v>0</v>
       </c>
       <c r="G164" t="n">
         <v>0</v>
@@ -4564,7 +4564,7 @@
         <v>0</v>
       </c>
       <c r="F165" t="n">
-        <v>1095</v>
+        <v>0</v>
       </c>
       <c r="G165" t="n">
         <v>0</v>
@@ -4589,7 +4589,7 @@
         <v>0</v>
       </c>
       <c r="F166" t="n">
-        <v>13938</v>
+        <v>0</v>
       </c>
       <c r="G166" t="n">
         <v>0</v>
@@ -4614,7 +4614,7 @@
         <v>0</v>
       </c>
       <c r="F167" t="n">
-        <v>9786</v>
+        <v>0</v>
       </c>
       <c r="G167" t="n">
         <v>0</v>
@@ -4639,10 +4639,10 @@
         <v>1608</v>
       </c>
       <c r="F168" t="n">
-        <v>6402</v>
+        <v>0</v>
       </c>
       <c r="G168" t="n">
-        <v>635</v>
+        <v>0</v>
       </c>
     </row>
     <row r="169">
@@ -4664,10 +4664,10 @@
         <v>2200</v>
       </c>
       <c r="F169" t="n">
-        <v>10074</v>
+        <v>0</v>
       </c>
       <c r="G169" t="n">
-        <v>1075</v>
+        <v>0</v>
       </c>
     </row>
     <row r="170">
@@ -4689,7 +4689,7 @@
         <v>0</v>
       </c>
       <c r="F170" t="n">
-        <v>6884</v>
+        <v>0</v>
       </c>
       <c r="G170" t="n">
         <v>0</v>
@@ -4714,7 +4714,7 @@
         <v>0</v>
       </c>
       <c r="F171" t="n">
-        <v>2846</v>
+        <v>0</v>
       </c>
       <c r="G171" t="n">
         <v>0</v>
@@ -4739,7 +4739,7 @@
         <v>0</v>
       </c>
       <c r="F172" t="n">
-        <v>6164</v>
+        <v>0</v>
       </c>
       <c r="G172" t="n">
         <v>0</v>
@@ -4764,10 +4764,10 @@
         <v>579</v>
       </c>
       <c r="F173" t="n">
-        <v>5865</v>
+        <v>0</v>
       </c>
       <c r="G173" t="n">
-        <v>238</v>
+        <v>0</v>
       </c>
     </row>
     <row r="174">
@@ -4789,7 +4789,7 @@
         <v>0</v>
       </c>
       <c r="F174" t="n">
-        <v>2246</v>
+        <v>0</v>
       </c>
       <c r="G174" t="n">
         <v>0</v>
@@ -4814,7 +4814,7 @@
         <v>0</v>
       </c>
       <c r="F175" t="n">
-        <v>3472</v>
+        <v>0</v>
       </c>
       <c r="G175" t="n">
         <v>0</v>
@@ -4839,10 +4839,10 @@
         <v>1319</v>
       </c>
       <c r="F176" t="n">
-        <v>7987</v>
+        <v>0</v>
       </c>
       <c r="G176" t="n">
-        <v>827</v>
+        <v>0</v>
       </c>
     </row>
     <row r="177">
@@ -4864,10 +4864,10 @@
         <v>941</v>
       </c>
       <c r="F177" t="n">
-        <v>9529</v>
+        <v>0</v>
       </c>
       <c r="G177" t="n">
-        <v>567</v>
+        <v>0</v>
       </c>
     </row>
     <row r="178">
@@ -4889,7 +4889,7 @@
         <v>0</v>
       </c>
       <c r="F178" t="n">
-        <v>4308</v>
+        <v>0</v>
       </c>
       <c r="G178" t="n">
         <v>0</v>
@@ -4914,7 +4914,7 @@
         <v>0</v>
       </c>
       <c r="F179" t="n">
-        <v>8024</v>
+        <v>0</v>
       </c>
       <c r="G179" t="n">
         <v>0</v>
@@ -4939,7 +4939,7 @@
         <v>0</v>
       </c>
       <c r="F180" t="n">
-        <v>9228</v>
+        <v>0</v>
       </c>
       <c r="G180" t="n">
         <v>0</v>
@@ -4964,7 +4964,7 @@
         <v>0</v>
       </c>
       <c r="F181" t="n">
-        <v>9319</v>
+        <v>0</v>
       </c>
       <c r="G181" t="n">
         <v>0</v>
@@ -4989,7 +4989,7 @@
         <v>0</v>
       </c>
       <c r="F182" t="n">
-        <v>5039</v>
+        <v>0</v>
       </c>
       <c r="G182" t="n">
         <v>0</v>
@@ -5014,10 +5014,10 @@
         <v>1691</v>
       </c>
       <c r="F183" t="n">
-        <v>3977</v>
+        <v>0</v>
       </c>
       <c r="G183" t="n">
-        <v>865</v>
+        <v>0</v>
       </c>
     </row>
     <row r="184">
@@ -5039,10 +5039,10 @@
         <v>4479</v>
       </c>
       <c r="F184" t="n">
-        <v>9897</v>
+        <v>0</v>
       </c>
       <c r="G184" t="n">
-        <v>2345</v>
+        <v>0</v>
       </c>
     </row>
     <row r="185">
@@ -5064,10 +5064,10 @@
         <v>1017</v>
       </c>
       <c r="F185" t="n">
-        <v>6673</v>
+        <v>0</v>
       </c>
       <c r="G185" t="n">
-        <v>604</v>
+        <v>0</v>
       </c>
     </row>
     <row r="186">
@@ -5089,7 +5089,7 @@
         <v>0</v>
       </c>
       <c r="F186" t="n">
-        <v>3703</v>
+        <v>0</v>
       </c>
       <c r="G186" t="n">
         <v>0</v>
@@ -5114,7 +5114,7 @@
         <v>0</v>
       </c>
       <c r="F187" t="n">
-        <v>4913</v>
+        <v>0</v>
       </c>
       <c r="G187" t="n">
         <v>0</v>
@@ -5139,7 +5139,7 @@
         <v>0</v>
       </c>
       <c r="F188" t="n">
-        <v>2120</v>
+        <v>0</v>
       </c>
       <c r="G188" t="n">
         <v>0</v>
@@ -5164,7 +5164,7 @@
         <v>0</v>
       </c>
       <c r="F189" t="n">
-        <v>5518</v>
+        <v>0</v>
       </c>
       <c r="G189" t="n">
         <v>0</v>
@@ -5189,7 +5189,7 @@
         <v>0</v>
       </c>
       <c r="F190" t="n">
-        <v>3431</v>
+        <v>0</v>
       </c>
       <c r="G190" t="n">
         <v>0</v>
@@ -5214,7 +5214,7 @@
         <v>0</v>
       </c>
       <c r="F191" t="n">
-        <v>4673</v>
+        <v>0</v>
       </c>
       <c r="G191" t="n">
         <v>0</v>
@@ -5239,7 +5239,7 @@
         <v>0</v>
       </c>
       <c r="F192" t="n">
-        <v>7023</v>
+        <v>0</v>
       </c>
       <c r="G192" t="n">
         <v>0</v>
@@ -5264,7 +5264,7 @@
         <v>0</v>
       </c>
       <c r="F193" t="n">
-        <v>9100</v>
+        <v>0</v>
       </c>
       <c r="G193" t="n">
         <v>0</v>
@@ -5289,7 +5289,7 @@
         <v>0</v>
       </c>
       <c r="F194" t="n">
-        <v>5985</v>
+        <v>0</v>
       </c>
       <c r="G194" t="n">
         <v>0</v>
@@ -5314,7 +5314,7 @@
         <v>0</v>
       </c>
       <c r="F195" t="n">
-        <v>6342</v>
+        <v>0</v>
       </c>
       <c r="G195" t="n">
         <v>0</v>
@@ -5339,7 +5339,7 @@
         <v>0</v>
       </c>
       <c r="F196" t="n">
-        <v>5208</v>
+        <v>0</v>
       </c>
       <c r="G196" t="n">
         <v>0</v>
@@ -5364,10 +5364,10 @@
         <v>2675</v>
       </c>
       <c r="F197" t="n">
-        <v>6684</v>
+        <v>0</v>
       </c>
       <c r="G197" t="n">
-        <v>1259</v>
+        <v>0</v>
       </c>
     </row>
     <row r="198">
@@ -5389,10 +5389,10 @@
         <v>4610</v>
       </c>
       <c r="F198" t="n">
-        <v>5179</v>
+        <v>0</v>
       </c>
       <c r="G198" t="n">
-        <v>1265</v>
+        <v>0</v>
       </c>
     </row>
     <row r="199">
@@ -5414,7 +5414,7 @@
         <v>0</v>
       </c>
       <c r="F199" t="n">
-        <v>2466</v>
+        <v>0</v>
       </c>
       <c r="G199" t="n">
         <v>0</v>
@@ -5439,7 +5439,7 @@
         <v>0</v>
       </c>
       <c r="F200" t="n">
-        <v>2491</v>
+        <v>0</v>
       </c>
       <c r="G200" t="n">
         <v>0</v>
@@ -5464,7 +5464,7 @@
         <v>0</v>
       </c>
       <c r="F201" t="n">
-        <v>3779</v>
+        <v>0</v>
       </c>
       <c r="G201" t="n">
         <v>0</v>
@@ -5489,7 +5489,7 @@
         <v>0</v>
       </c>
       <c r="F202" t="n">
-        <v>3278</v>
+        <v>0</v>
       </c>
       <c r="G202" t="n">
         <v>0</v>
@@ -5514,10 +5514,10 @@
         <v>396</v>
       </c>
       <c r="F203" t="n">
-        <v>3691</v>
+        <v>0</v>
       </c>
       <c r="G203" t="n">
-        <v>136</v>
+        <v>0</v>
       </c>
     </row>
     <row r="204">
@@ -5539,7 +5539,7 @@
         <v>0</v>
       </c>
       <c r="F204" t="n">
-        <v>4635</v>
+        <v>0</v>
       </c>
       <c r="G204" t="n">
         <v>0</v>
@@ -5564,7 +5564,7 @@
         <v>0</v>
       </c>
       <c r="F205" t="n">
-        <v>4664</v>
+        <v>0</v>
       </c>
       <c r="G205" t="n">
         <v>0</v>
@@ -5589,7 +5589,7 @@
         <v>0</v>
       </c>
       <c r="F206" t="n">
-        <v>6453</v>
+        <v>0</v>
       </c>
       <c r="G206" t="n">
         <v>0</v>
@@ -5614,10 +5614,10 @@
         <v>2636</v>
       </c>
       <c r="F207" t="n">
-        <v>4542</v>
+        <v>0</v>
       </c>
       <c r="G207" t="n">
-        <v>1356</v>
+        <v>0</v>
       </c>
     </row>
     <row r="208">
@@ -5639,7 +5639,7 @@
         <v>0</v>
       </c>
       <c r="F208" t="n">
-        <v>5600</v>
+        <v>0</v>
       </c>
       <c r="G208" t="n">
         <v>0</v>
@@ -5664,10 +5664,10 @@
         <v>61</v>
       </c>
       <c r="F209" t="n">
-        <v>4356</v>
+        <v>0</v>
       </c>
       <c r="G209" t="n">
-        <v>63</v>
+        <v>0</v>
       </c>
     </row>
     <row r="210">
@@ -5689,7 +5689,7 @@
         <v>0</v>
       </c>
       <c r="F210" t="n">
-        <v>4848</v>
+        <v>0</v>
       </c>
       <c r="G210" t="n">
         <v>0</v>
@@ -5714,7 +5714,7 @@
         <v>0</v>
       </c>
       <c r="F211" t="n">
-        <v>6621</v>
+        <v>0</v>
       </c>
       <c r="G211" t="n">
         <v>0</v>
@@ -5739,7 +5739,7 @@
         <v>0</v>
       </c>
       <c r="F212" t="n">
-        <v>4474</v>
+        <v>0</v>
       </c>
       <c r="G212" t="n">
         <v>0</v>
@@ -5764,7 +5764,7 @@
         <v>0</v>
       </c>
       <c r="F213" t="n">
-        <v>1187</v>
+        <v>0</v>
       </c>
       <c r="G213" t="n">
         <v>0</v>

</xml_diff>